<commit_message>
typo in input.xlsx fixed
</commit_message>
<xml_diff>
--- a/examples/specficationSheets/Input.xlsx
+++ b/examples/specficationSheets/Input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ednaruckhaus/Documents/GitHub/Mapeathor/examples/specficationSheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiglesias/PycharmProjects/Mapeathor/examples/specficationSheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7450EF-77C7-634A-A1D2-75EF786B55A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E702F1FC-CE1A-CF4D-9D7B-21B818F08C6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26300" windowHeight="15600" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26300" windowHeight="15600" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefixes" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="80">
   <si>
     <t>Prefix</t>
   </si>
@@ -140,9 +140,6 @@
   </si>
   <si>
     <t>data/clasificacion-economica-gasto-madrid.csv</t>
-  </si>
-  <si>
-    <t>clasificacion-economica-gasto-madrid.csv</t>
   </si>
   <si>
     <t>IdGastoCentro</t>
@@ -758,7 +755,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" t="s">
         <v>24</v>
@@ -766,7 +763,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
         <v>25</v>
@@ -774,7 +771,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B15" t="s">
         <v>26</v>
@@ -805,7 +802,7 @@
         <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -816,10 +813,10 @@
         <v>30</v>
       </c>
       <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
         <v>42</v>
-      </c>
-      <c r="C2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -827,43 +824,43 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
         <v>44</v>
-      </c>
-      <c r="C3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -876,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -938,12 +935,12 @@
         <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
         <v>31</v>
@@ -954,7 +951,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
         <v>33</v>
@@ -965,7 +962,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
         <v>31</v>
@@ -976,7 +973,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
         <v>33</v>
@@ -987,7 +984,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
         <v>31</v>
@@ -998,7 +995,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
         <v>33</v>
@@ -1017,7 +1014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -1035,22 +1032,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>27</v>
@@ -1058,13 +1055,13 @@
     </row>
     <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" t="s">
         <v>56</v>
-      </c>
-      <c r="C2" t="s">
-        <v>57</v>
       </c>
       <c r="G2" t="s">
         <v>30</v>
@@ -1072,13 +1069,13 @@
     </row>
     <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
         <v>58</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" t="s">
-        <v>59</v>
       </c>
       <c r="G3" t="s">
         <v>30</v>
@@ -1086,13 +1083,13 @@
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G4" t="s">
         <v>30</v>
@@ -1100,20 +1097,20 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
         <v>35</v>
       </c>
       <c r="E5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" t="s">
         <v>63</v>
-      </c>
-      <c r="F5" t="s">
-        <v>64</v>
       </c>
       <c r="G5" t="s">
         <v>30</v>
@@ -1121,13 +1118,13 @@
     </row>
     <row r="6" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>35</v>
@@ -1135,13 +1132,13 @@
     </row>
     <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" t="s">
         <v>68</v>
-      </c>
-      <c r="C7" t="s">
-        <v>69</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>35</v>
@@ -1149,114 +1146,114 @@
     </row>
     <row r="8" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1281,13 +1278,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>